<commit_message>
Splitting Client, update build script
</commit_message>
<xml_diff>
--- a/database/majors.xlsx
+++ b/database/majors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\design_tool\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\doc_automation\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22DC3876-33FC-4994-9C3F-302BA4BBB2C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FC4FDE-2B4B-46CC-B39B-3226D2154312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2115" yWindow="2115" windowWidth="16200" windowHeight="9983" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,59 +25,47 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>学院甲</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>生物专业</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>不知道干啥的专业</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>学院2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>学院3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>哈哈哈专业</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>嘻嘻嘻专业</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>咕咕咕专业</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>呼噜噜专业</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>信息与通信工程学院</t>
+  </si>
+  <si>
+    <t>通信工程</t>
+  </si>
+  <si>
+    <t>电子信息工程</t>
+  </si>
+  <si>
+    <t>广播电视工程（智能视听技术方向）</t>
+  </si>
+  <si>
+    <t>数字媒体技术</t>
+  </si>
+  <si>
+    <t>物联网工程</t>
+  </si>
+  <si>
+    <t>人工智能</t>
+  </si>
+  <si>
+    <t>智能装备系统（演艺工程与智能技术方向）</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -107,7 +95,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -385,47 +373,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="168" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="168" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>